<commit_message>
update policies data download files, with sources
</commit_message>
<xml_diff>
--- a/data/download/California Prison Population - Two Strike Policy.xlsx
+++ b/data/download/California Prison Population - Two Strike Policy.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\EPelletier\Box Sync\09126 OSF Long Sentences\Data\Final\DOWNLOADABLE DATA FILES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\LCourtney\Box Sync\09126 OSF Long Sentences\Website Content\Policy section\Final Excel sheets for website\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9675"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>California Prison Population - Two Strikes Policy</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Total Prison Population</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>http://www.cdcr.ca.gov/Reports_Research/Offender_Information_Services_Branch/Quarterly/Strike1Archive.html</t>
+  </si>
+  <si>
+    <t>California Department of Corrections and Rehabilitation: Second and Third Strike Inmate Population Report Archive</t>
   </si>
 </sst>
 </file>
@@ -397,23 +406,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.21875" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -421,7 +430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2006</v>
       </c>
@@ -432,7 +441,7 @@
         <v>173101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2016</v>
       </c>
@@ -443,7 +452,23 @@
         <v>129105</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>